<commit_message>
added changes to package names, scrape VOs, scrapeadaptors
</commit_message>
<xml_diff>
--- a/ScrapeAnalysis/DataScraperAnalysis/Spec Examples.xlsx
+++ b/ScrapeAnalysis/DataScraperAnalysis/Spec Examples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="15150" windowHeight="7980"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="15150" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scraper Error XML" sheetId="7" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Scraper attempts to scrape with invalid user credentials</t>
   </si>
@@ -381,9 +381,50 @@
   &lt;time&gt;13:50:00&lt;/time&gt;
   &lt;datapair id="001"&gt;
     &lt;text&gt;Scraper Error&lt;/text&gt;
-    &lt;value&gt;UndeterminedError&lt;/value&gt;
+    &lt;value&gt;ErrorPageEncountered&lt;/value&gt;
   &lt;/datapair&gt;
 &lt;/scrape-session&gt;</t>
+  </si>
+  <si>
+    <t>Scraper attempts to scraped website that has error page displayed as a result of intermittent circumstances</t>
+  </si>
+  <si>
+    <t>Error Code</t>
+  </si>
+  <si>
+    <t>InvalidCredentials</t>
+  </si>
+  <si>
+    <t>UserNotSignedUpForEbilling</t>
+  </si>
+  <si>
+    <t>AccountUpdateRequired</t>
+  </si>
+  <si>
+    <t>BillingSiteDown</t>
+  </si>
+  <si>
+    <t>BillingSitePageError</t>
+  </si>
+  <si>
+    <t>ErrorPageEncountered</t>
+  </si>
+  <si>
+    <t>&lt;scrape-session&gt;
+  &lt;baseURL&gt;www.elen7045.co.za&lt;/baseURL&gt;
+  &lt;date&gt;12/12/2014&lt;/date&gt;
+  &lt;time&gt;13:50:00&lt;/time&gt;
+  &lt;datapair id="001"&gt;
+    &lt;text&gt;Scraper Error&lt;/text&gt;
+    &lt;value&gt;BrokenScript&lt;/value&gt;
+  &lt;/datapair&gt;
+&lt;/scrape-session&gt;</t>
+  </si>
+  <si>
+    <t>BrokenScript</t>
+  </si>
+  <si>
+    <t>000</t>
   </si>
 </sst>
 </file>
@@ -442,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -460,8 +501,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -777,63 +827,89 @@
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C1" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" spans="1:3" ht="151.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="79.5" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="75.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="77.25" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" ht="80.25" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="C6" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="77.25" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="80.25" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1"/>
+      <c r="B8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" s="6"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1"/>
@@ -849,6 +925,9 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -858,48 +937,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="161.25" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="C1" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="161.25" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="141" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="C2" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="141" customHeight="1">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="142.5" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="C3" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="142.5" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>